<commit_message>
Add generated JSON files
</commit_message>
<xml_diff>
--- a/src/files/workflow_files/now_price8.xlsx
+++ b/src/files/workflow_files/now_price8.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6.30</t>
+          <t>6.43</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>73.08</t>
+          <t>72.09</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>13.44</t>
+          <t>13.31</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>17.33</t>
+          <t>17.40</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>41.93</t>
+          <t>42.39</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1493.72</t>
+          <t>1488.11</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>354.49</t>
+          <t>360.67</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10.80</t>
+          <t>10.75</t>
         </is>
       </c>
     </row>

</xml_diff>